<commit_message>
reclassed problem as 3 class and reran setfit
</commit_message>
<xml_diff>
--- a/results/overview/summary_all_F1.xlsx
+++ b/results/overview/summary_all_F1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,313 +436,356 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>reddit</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>patio_lawn_garden</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>twitter</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>lidl</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>automotive</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ikea_reviews</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>luxury_beauty</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>instant_video</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>twitter</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>automotive</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>luxury_beauty</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>patio_lawn_garden</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>musical_instruments</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>reddit</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>office_products</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>ikea_reviews</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>hotel</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>drugs</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>lidl</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>RF</t>
+          <t>ComplementNB</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>41.86</v>
+        <v>66.95999999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>56.07</v>
+        <v>50.43</v>
       </c>
       <c r="D2" t="n">
-        <v>54.25</v>
+        <v>78.01000000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>52.91</v>
+        <v>64.09999999999999</v>
       </c>
       <c r="F2" t="n">
-        <v>37.53</v>
+        <v>60.71</v>
       </c>
       <c r="G2" t="n">
-        <v>55.15</v>
+        <v>66.39</v>
       </c>
       <c r="H2" t="n">
-        <v>61.4</v>
+        <v>67.42</v>
       </c>
       <c r="I2" t="n">
-        <v>41.09</v>
+        <v>56.23</v>
       </c>
       <c r="J2" t="n">
-        <v>60.46</v>
+        <v>58.72</v>
       </c>
       <c r="K2" t="n">
-        <v>31.84</v>
+        <v>56.27</v>
       </c>
       <c r="L2" t="n">
-        <v>17.92</v>
+        <v>50.16</v>
       </c>
       <c r="M2" t="n">
-        <v>51.33</v>
+        <v>37.83</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>ComplementNB</t>
+          <t>Decision Tree</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>56.31</v>
+        <v>60.37</v>
       </c>
       <c r="C3" t="n">
-        <v>77.93000000000001</v>
+        <v>42.8</v>
       </c>
       <c r="D3" t="n">
-        <v>61.6</v>
+        <v>67.69</v>
       </c>
       <c r="E3" t="n">
-        <v>67.3</v>
+        <v>58.7</v>
       </c>
       <c r="F3" t="n">
-        <v>50.01</v>
+        <v>55.36</v>
       </c>
       <c r="G3" t="n">
-        <v>60.54</v>
+        <v>60.76</v>
       </c>
       <c r="H3" t="n">
-        <v>67.27</v>
+        <v>64.52</v>
       </c>
       <c r="I3" t="n">
-        <v>56.41</v>
+        <v>45.84</v>
       </c>
       <c r="J3" t="n">
-        <v>66.84999999999999</v>
+        <v>56.07</v>
       </c>
       <c r="K3" t="n">
-        <v>49.91</v>
+        <v>46.38</v>
       </c>
       <c r="L3" t="n">
-        <v>37.83</v>
+        <v>39.48</v>
       </c>
       <c r="M3" t="n">
-        <v>64.22</v>
+        <v>33.99</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Decision Tree</t>
+          <t>LR</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>45.84</v>
+        <v>70.39</v>
       </c>
       <c r="C4" t="n">
-        <v>67.69</v>
+        <v>54.35</v>
       </c>
       <c r="D4" t="n">
-        <v>55.36</v>
+        <v>80.56</v>
       </c>
       <c r="E4" t="n">
-        <v>64.52</v>
+        <v>66.41</v>
       </c>
       <c r="F4" t="n">
-        <v>42.8</v>
+        <v>62.39</v>
       </c>
       <c r="G4" t="n">
-        <v>56.07</v>
+        <v>71.14</v>
       </c>
       <c r="H4" t="n">
-        <v>60.37</v>
+        <v>73.23</v>
       </c>
       <c r="I4" t="n">
-        <v>46.38</v>
+        <v>59.57</v>
       </c>
       <c r="J4" t="n">
-        <v>60.76</v>
+        <v>62.56</v>
       </c>
       <c r="K4" t="n">
-        <v>39.48</v>
+        <v>61.17</v>
       </c>
       <c r="L4" t="n">
-        <v>33.99</v>
+        <v>52.19</v>
       </c>
       <c r="M4" t="n">
-        <v>58.7</v>
+        <v>42.32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>LR</t>
+          <t>MultinomialNB</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>59.57</v>
+        <v>67.16</v>
       </c>
       <c r="C5" t="n">
-        <v>80.56</v>
+        <v>47.1</v>
       </c>
       <c r="D5" t="n">
-        <v>62.39</v>
+        <v>73.43000000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>73.23</v>
+        <v>64.54000000000001</v>
       </c>
       <c r="F5" t="n">
-        <v>54.35</v>
+        <v>56.83</v>
       </c>
       <c r="G5" t="n">
-        <v>62.56</v>
+        <v>69.14</v>
       </c>
       <c r="H5" t="n">
-        <v>70.39</v>
+        <v>63.67</v>
       </c>
       <c r="I5" t="n">
-        <v>61.17</v>
+        <v>51.3</v>
       </c>
       <c r="J5" t="n">
-        <v>71.14</v>
+        <v>56.52</v>
       </c>
       <c r="K5" t="n">
-        <v>52.19</v>
+        <v>50.13</v>
       </c>
       <c r="L5" t="n">
-        <v>42.32</v>
+        <v>49.11</v>
       </c>
       <c r="M5" t="n">
-        <v>66.41</v>
+        <v>35.52</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MultinomialNB</t>
+          <t>RF</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>51.3</v>
+        <v>61.4</v>
       </c>
       <c r="C6" t="n">
-        <v>73.43000000000001</v>
+        <v>37.53</v>
       </c>
       <c r="D6" t="n">
-        <v>56.83</v>
+        <v>56.07</v>
       </c>
       <c r="E6" t="n">
-        <v>63.67</v>
+        <v>51.33</v>
       </c>
       <c r="F6" t="n">
-        <v>47.1</v>
+        <v>54.25</v>
       </c>
       <c r="G6" t="n">
-        <v>56.52</v>
+        <v>60.46</v>
       </c>
       <c r="H6" t="n">
-        <v>67.16</v>
+        <v>52.91</v>
       </c>
       <c r="I6" t="n">
-        <v>50.13</v>
+        <v>41.86</v>
       </c>
       <c r="J6" t="n">
-        <v>69.14</v>
+        <v>55.15</v>
       </c>
       <c r="K6" t="n">
-        <v>49.11</v>
+        <v>41.09</v>
       </c>
       <c r="L6" t="n">
-        <v>35.52</v>
+        <v>31.84</v>
       </c>
       <c r="M6" t="n">
-        <v>64.54000000000001</v>
+        <v>17.92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
+          <t>setfit</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>58.99</v>
+      </c>
+      <c r="C7" t="n">
+        <v>63.57</v>
+      </c>
+      <c r="D7" t="n">
+        <v>73.31999999999999</v>
+      </c>
+      <c r="E7" t="n">
+        <v>53.21</v>
+      </c>
+      <c r="F7" t="n">
+        <v>59.24</v>
+      </c>
+      <c r="G7" t="n">
+        <v>67.37</v>
+      </c>
+      <c r="H7" t="n">
+        <v>69.56</v>
+      </c>
+      <c r="I7" t="n">
+        <v>67.06</v>
+      </c>
+      <c r="J7" t="n">
+        <v>73.31999999999999</v>
+      </c>
+      <c r="K7" t="n">
+        <v>68.11</v>
+      </c>
+      <c r="L7" t="n">
+        <v>71.06999999999999</v>
+      </c>
+      <c r="M7" t="n">
+        <v>58.61</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
           <t>SVM</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>67.38</v>
+      </c>
+      <c r="F8" t="n">
+        <v>64.64</v>
+      </c>
+      <c r="G8" t="n">
+        <v>70.33</v>
+      </c>
+      <c r="H8" t="n">
+        <v>75.09999999999999</v>
+      </c>
+      <c r="I8" t="n">
         <v>59.99</v>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="n">
-        <v>64.64</v>
-      </c>
-      <c r="E7" t="n">
-        <v>75.09999999999999</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
+      <c r="J8" t="n">
         <v>61.56</v>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="n">
-        <v>70.33</v>
-      </c>
-      <c r="K7" t="n">
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="n">
         <v>53.67</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M8" t="n">
         <v>46.73</v>
-      </c>
-      <c r="M7" t="n">
-        <v>67.38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>